<commit_message>
1.6.0 adding a force_pick, add_team, and remove_team to the admin commands
</commit_message>
<xml_diff>
--- a/excels/Valley Mall 2025_draft.xlsx
+++ b/excels/Valley Mall 2025_draft.xlsx
@@ -467,7 +467,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
@@ -506,7 +506,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Jerry || 20850Z</t>
+          <t>Aidan || 7135Z</t>
         </is>
       </c>
       <c r="B2" s="2" t="n"/>
@@ -517,7 +517,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Aidan || 7135Z</t>
+          <t>Michael || 676D</t>
         </is>
       </c>
       <c r="B3" s="2" t="n"/>
@@ -528,7 +528,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Rowan || 593C</t>
+          <t>Jeremiah || OBSR || 676V</t>
         </is>
       </c>
       <c r="B4" s="2" t="n"/>
@@ -539,7 +539,7 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Jeremiah || OBSR || 676V</t>
+          <t>Edward || 929</t>
         </is>
       </c>
       <c r="B5" s="2" t="n"/>
@@ -550,7 +550,7 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>James || 9080S</t>
+          <t>Donald || 20850V</t>
         </is>
       </c>
       <c r="B6" s="2" t="n"/>
@@ -561,7 +561,7 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Amelia || 20850A</t>
+          <t>Charlie || 929K</t>
         </is>
       </c>
       <c r="B7" s="2" t="n"/>
@@ -572,7 +572,7 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Jack || 934Z</t>
+          <t>Jerry || 20850Z</t>
         </is>
       </c>
       <c r="B8" s="2" t="n"/>
@@ -583,7 +583,7 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Michael || 676D</t>
+          <t>Rowan || 593C</t>
         </is>
       </c>
       <c r="B9" s="2" t="n"/>
@@ -594,7 +594,7 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Chad || 53E</t>
+          <t>James || 9080S</t>
         </is>
       </c>
       <c r="B10" s="2" t="n"/>
@@ -605,7 +605,7 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Leah || 929T</t>
+          <t>Jack || 934Z</t>
         </is>
       </c>
       <c r="B11" s="2" t="n"/>
@@ -616,7 +616,7 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Edward || 929</t>
+          <t>Leah || 929T</t>
         </is>
       </c>
       <c r="B12" s="2" t="n"/>
@@ -627,7 +627,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Donald || 20850V</t>
+          <t>Chad || 53E</t>
         </is>
       </c>
       <c r="B13" s="2" t="n"/>
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Charlie || 929K</t>
+          <t>Amelia || 20850A</t>
         </is>
       </c>
       <c r="B14" s="2" t="n"/>

</xml_diff>